<commit_message>
adding tests for problems
</commit_message>
<xml_diff>
--- a/src/PeStopAnnualReport/data/centralizare_pe_stop.xlsx
+++ b/src/PeStopAnnualReport/data/centralizare_pe_stop.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eu\GitHub\PeStop\src\PeStopAnnualReport\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FB8B9AD-4E88-488B-9217-08F8FCD643B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84F71FE4-6A21-4D24-A7CF-D85F8802C686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -383,7 +383,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -565,9 +565,7 @@
       <c r="D10" s="1">
         <v>48</v>
       </c>
-      <c r="E10" s="1">
-        <v>50</v>
-      </c>
+      <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="1">
@@ -595,7 +593,6 @@
         <v>15</v>
       </c>
       <c r="C12" s="1">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("importrange(""https://docs.google.com/spreadsheets/d/1_euHfeY7S3jgqXK1kAnatxKzNaPplzMUordedR37MTM/edit?gid=0#gid=0"",""Noiembrie 2025!G1"")"),0)</f>
         <v>0</v>
       </c>
       <c r="D12" s="1">

</xml_diff>